<commit_message>
Fixed the naviation typo. All 'naviation' in CEDS has been changed to 'navigation'.
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/Europe and other Heavy Oil S.xlsx
+++ b/input/default-emissions-data/Europe and other Heavy Oil S.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24660" windowHeight="10920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="31400" windowHeight="17920" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input-tab" sheetId="2" r:id="rId1"/>
@@ -201,9 +201,6 @@
     <t>1A3c_Rail</t>
   </si>
   <si>
-    <t>1A3dii_Domestic-naviation</t>
-  </si>
-  <si>
     <t>1A4a_Commercial-institutional</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>Keep constant from 1960 - 1980 so won't increase before 1980</t>
+  </si>
+  <si>
+    <t>1A3dii_Domestic-navigation</t>
   </si>
 </sst>
 </file>
@@ -978,7 +978,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:I3"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -20295,7 +20295,7 @@
       </c>
       <c r="B537" t="str">
         <f>'Europe-Calc'!B536</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C537" t="s">
         <v>2</v>
@@ -20331,7 +20331,7 @@
       </c>
       <c r="B538" t="str">
         <f>'Europe-Calc'!B537</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C538" t="s">
         <v>2</v>
@@ -20367,7 +20367,7 @@
       </c>
       <c r="B539" t="str">
         <f>'Europe-Calc'!B538</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C539" t="s">
         <v>2</v>
@@ -20403,7 +20403,7 @@
       </c>
       <c r="B540" t="str">
         <f>'Europe-Calc'!B539</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C540" t="s">
         <v>2</v>
@@ -20439,7 +20439,7 @@
       </c>
       <c r="B541" t="str">
         <f>'Europe-Calc'!B540</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C541" t="s">
         <v>2</v>
@@ -20475,7 +20475,7 @@
       </c>
       <c r="B542" t="str">
         <f>'Europe-Calc'!B541</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C542" t="s">
         <v>2</v>
@@ -20511,7 +20511,7 @@
       </c>
       <c r="B543" t="str">
         <f>'Europe-Calc'!B542</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C543" t="s">
         <v>2</v>
@@ -20547,7 +20547,7 @@
       </c>
       <c r="B544" t="str">
         <f>'Europe-Calc'!B543</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C544" t="s">
         <v>2</v>
@@ -20583,7 +20583,7 @@
       </c>
       <c r="B545" t="str">
         <f>'Europe-Calc'!B544</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C545" t="s">
         <v>2</v>
@@ -20619,7 +20619,7 @@
       </c>
       <c r="B546" t="str">
         <f>'Europe-Calc'!B545</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C546" t="s">
         <v>2</v>
@@ -20655,7 +20655,7 @@
       </c>
       <c r="B547" t="str">
         <f>'Europe-Calc'!B546</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C547" t="s">
         <v>2</v>
@@ -20691,7 +20691,7 @@
       </c>
       <c r="B548" t="str">
         <f>'Europe-Calc'!B547</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C548" t="s">
         <v>2</v>
@@ -20727,7 +20727,7 @@
       </c>
       <c r="B549" t="str">
         <f>'Europe-Calc'!B548</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C549" t="s">
         <v>2</v>
@@ -20763,7 +20763,7 @@
       </c>
       <c r="B550" t="str">
         <f>'Europe-Calc'!B549</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C550" t="s">
         <v>2</v>
@@ -20799,7 +20799,7 @@
       </c>
       <c r="B551" t="str">
         <f>'Europe-Calc'!B550</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C551" t="s">
         <v>2</v>
@@ -20835,7 +20835,7 @@
       </c>
       <c r="B552" t="str">
         <f>'Europe-Calc'!B551</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C552" t="s">
         <v>2</v>
@@ -20871,7 +20871,7 @@
       </c>
       <c r="B553" t="str">
         <f>'Europe-Calc'!B552</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C553" t="s">
         <v>2</v>
@@ -20907,7 +20907,7 @@
       </c>
       <c r="B554" t="str">
         <f>'Europe-Calc'!B553</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C554" t="s">
         <v>2</v>
@@ -20943,7 +20943,7 @@
       </c>
       <c r="B555" t="str">
         <f>'Europe-Calc'!B554</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C555" t="s">
         <v>2</v>
@@ -20979,7 +20979,7 @@
       </c>
       <c r="B556" t="str">
         <f>'Europe-Calc'!B555</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C556" t="s">
         <v>2</v>
@@ -21015,7 +21015,7 @@
       </c>
       <c r="B557" t="str">
         <f>'Europe-Calc'!B556</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C557" t="s">
         <v>2</v>
@@ -21051,7 +21051,7 @@
       </c>
       <c r="B558" t="str">
         <f>'Europe-Calc'!B557</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C558" t="s">
         <v>2</v>
@@ -21087,7 +21087,7 @@
       </c>
       <c r="B559" t="str">
         <f>'Europe-Calc'!B558</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C559" t="s">
         <v>2</v>
@@ -21123,7 +21123,7 @@
       </c>
       <c r="B560" t="str">
         <f>'Europe-Calc'!B559</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C560" t="s">
         <v>2</v>
@@ -21159,7 +21159,7 @@
       </c>
       <c r="B561" t="str">
         <f>'Europe-Calc'!B560</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C561" t="s">
         <v>2</v>
@@ -21195,7 +21195,7 @@
       </c>
       <c r="B562" t="str">
         <f>'Europe-Calc'!B561</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C562" t="s">
         <v>2</v>
@@ -21231,7 +21231,7 @@
       </c>
       <c r="B563" t="str">
         <f>'Europe-Calc'!B562</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C563" t="s">
         <v>2</v>
@@ -21267,7 +21267,7 @@
       </c>
       <c r="B564" t="str">
         <f>'Europe-Calc'!B563</f>
-        <v>1A3dii_Domestic-naviation</v>
+        <v>1A3dii_Domestic-navigation</v>
       </c>
       <c r="C564" t="s">
         <v>2</v>
@@ -25343,11 +25343,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N675"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E536" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J69" sqref="A1:K675"/>
+      <selection pane="bottomRight" activeCell="B563" sqref="B563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -25364,7 +25364,7 @@
         <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -25396,13 +25396,13 @@
         <v>2005</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -27664,7 +27664,7 @@
         <v>2.6723334840000001E-2</v>
       </c>
       <c r="J69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -27697,7 +27697,7 @@
         <v>2.6723334840000001E-2</v>
       </c>
       <c r="J70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -27730,7 +27730,7 @@
         <v>2.6723334840000001E-2</v>
       </c>
       <c r="J71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -27766,7 +27766,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
       <c r="J72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -28692,7 +28692,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J100" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -42498,7 +42498,7 @@
         <v>0.01</v>
       </c>
       <c r="K508" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="509" spans="1:11">
@@ -43370,7 +43370,7 @@
         <v>0</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C536" s="2" t="s">
         <v>2</v>
@@ -43402,7 +43402,7 @@
         <v>4</v>
       </c>
       <c r="B537" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C537" s="4" t="s">
         <v>2</v>
@@ -43434,7 +43434,7 @@
         <v>5</v>
       </c>
       <c r="B538" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C538" s="4" t="s">
         <v>2</v>
@@ -43466,7 +43466,7 @@
         <v>6</v>
       </c>
       <c r="B539" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C539" s="4" t="s">
         <v>2</v>
@@ -43498,7 +43498,7 @@
         <v>7</v>
       </c>
       <c r="B540" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C540" s="4" t="s">
         <v>2</v>
@@ -43530,7 +43530,7 @@
         <v>8</v>
       </c>
       <c r="B541" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C541" s="4" t="s">
         <v>2</v>
@@ -43562,7 +43562,7 @@
         <v>9</v>
       </c>
       <c r="B542" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C542" s="4" t="s">
         <v>2</v>
@@ -43594,7 +43594,7 @@
         <v>10</v>
       </c>
       <c r="B543" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C543" s="4" t="s">
         <v>2</v>
@@ -43626,7 +43626,7 @@
         <v>11</v>
       </c>
       <c r="B544" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C544" s="4" t="s">
         <v>2</v>
@@ -43658,7 +43658,7 @@
         <v>12</v>
       </c>
       <c r="B545" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C545" s="4" t="s">
         <v>2</v>
@@ -43690,7 +43690,7 @@
         <v>13</v>
       </c>
       <c r="B546" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C546" s="4" t="s">
         <v>2</v>
@@ -43722,7 +43722,7 @@
         <v>14</v>
       </c>
       <c r="B547" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C547" s="4" t="s">
         <v>2</v>
@@ -43754,7 +43754,7 @@
         <v>15</v>
       </c>
       <c r="B548" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C548" s="4" t="s">
         <v>2</v>
@@ -43786,7 +43786,7 @@
         <v>16</v>
       </c>
       <c r="B549" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C549" s="4" t="s">
         <v>2</v>
@@ -43818,7 +43818,7 @@
         <v>17</v>
       </c>
       <c r="B550" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C550" s="4" t="s">
         <v>2</v>
@@ -43850,7 +43850,7 @@
         <v>18</v>
       </c>
       <c r="B551" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C551" s="4" t="s">
         <v>2</v>
@@ -43882,7 +43882,7 @@
         <v>19</v>
       </c>
       <c r="B552" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C552" s="4" t="s">
         <v>2</v>
@@ -43914,7 +43914,7 @@
         <v>20</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C553" s="4" t="s">
         <v>2</v>
@@ -43946,7 +43946,7 @@
         <v>21</v>
       </c>
       <c r="B554" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C554" s="4" t="s">
         <v>2</v>
@@ -43978,7 +43978,7 @@
         <v>22</v>
       </c>
       <c r="B555" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C555" s="4" t="s">
         <v>2</v>
@@ -44010,7 +44010,7 @@
         <v>23</v>
       </c>
       <c r="B556" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C556" s="4" t="s">
         <v>2</v>
@@ -44042,7 +44042,7 @@
         <v>24</v>
       </c>
       <c r="B557" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C557" s="4" t="s">
         <v>2</v>
@@ -44074,7 +44074,7 @@
         <v>25</v>
       </c>
       <c r="B558" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C558" s="4" t="s">
         <v>2</v>
@@ -44106,7 +44106,7 @@
         <v>26</v>
       </c>
       <c r="B559" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C559" s="4" t="s">
         <v>2</v>
@@ -44138,7 +44138,7 @@
         <v>27</v>
       </c>
       <c r="B560" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C560" s="4" t="s">
         <v>2</v>
@@ -44170,7 +44170,7 @@
         <v>28</v>
       </c>
       <c r="B561" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C561" s="4" t="s">
         <v>2</v>
@@ -44202,7 +44202,7 @@
         <v>29</v>
       </c>
       <c r="B562" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C562" s="4" t="s">
         <v>2</v>
@@ -44234,7 +44234,7 @@
         <v>30</v>
       </c>
       <c r="B563" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C563" s="4" t="s">
         <v>2</v>
@@ -44266,7 +44266,7 @@
         <v>0</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C564" s="2" t="s">
         <v>2</v>
@@ -44298,7 +44298,7 @@
         <v>4</v>
       </c>
       <c r="B565" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C565" s="4" t="s">
         <v>2</v>
@@ -44330,7 +44330,7 @@
         <v>5</v>
       </c>
       <c r="B566" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C566" s="4" t="s">
         <v>2</v>
@@ -44362,7 +44362,7 @@
         <v>6</v>
       </c>
       <c r="B567" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C567" s="4" t="s">
         <v>2</v>
@@ -44394,7 +44394,7 @@
         <v>7</v>
       </c>
       <c r="B568" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C568" s="4" t="s">
         <v>2</v>
@@ -44426,7 +44426,7 @@
         <v>8</v>
       </c>
       <c r="B569" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C569" s="4" t="s">
         <v>2</v>
@@ -44458,7 +44458,7 @@
         <v>9</v>
       </c>
       <c r="B570" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C570" s="4" t="s">
         <v>2</v>
@@ -44490,7 +44490,7 @@
         <v>10</v>
       </c>
       <c r="B571" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C571" s="4" t="s">
         <v>2</v>
@@ -44522,7 +44522,7 @@
         <v>11</v>
       </c>
       <c r="B572" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C572" s="4" t="s">
         <v>2</v>
@@ -44554,7 +44554,7 @@
         <v>12</v>
       </c>
       <c r="B573" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C573" s="4" t="s">
         <v>2</v>
@@ -44586,7 +44586,7 @@
         <v>13</v>
       </c>
       <c r="B574" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C574" s="4" t="s">
         <v>2</v>
@@ -44618,7 +44618,7 @@
         <v>14</v>
       </c>
       <c r="B575" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C575" s="4" t="s">
         <v>2</v>
@@ -44650,7 +44650,7 @@
         <v>15</v>
       </c>
       <c r="B576" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C576" s="4" t="s">
         <v>2</v>
@@ -44682,7 +44682,7 @@
         <v>16</v>
       </c>
       <c r="B577" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C577" s="4" t="s">
         <v>2</v>
@@ -44714,7 +44714,7 @@
         <v>17</v>
       </c>
       <c r="B578" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C578" s="4" t="s">
         <v>2</v>
@@ -44746,7 +44746,7 @@
         <v>18</v>
       </c>
       <c r="B579" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C579" s="4" t="s">
         <v>2</v>
@@ -44778,7 +44778,7 @@
         <v>19</v>
       </c>
       <c r="B580" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C580" s="4" t="s">
         <v>2</v>
@@ -44810,7 +44810,7 @@
         <v>20</v>
       </c>
       <c r="B581" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C581" s="4" t="s">
         <v>2</v>
@@ -44842,7 +44842,7 @@
         <v>21</v>
       </c>
       <c r="B582" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C582" s="4" t="s">
         <v>2</v>
@@ -44874,7 +44874,7 @@
         <v>22</v>
       </c>
       <c r="B583" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C583" s="4" t="s">
         <v>2</v>
@@ -44906,7 +44906,7 @@
         <v>23</v>
       </c>
       <c r="B584" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C584" s="4" t="s">
         <v>2</v>
@@ -44938,7 +44938,7 @@
         <v>24</v>
       </c>
       <c r="B585" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C585" s="4" t="s">
         <v>2</v>
@@ -44970,7 +44970,7 @@
         <v>25</v>
       </c>
       <c r="B586" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C586" s="4" t="s">
         <v>2</v>
@@ -45002,7 +45002,7 @@
         <v>26</v>
       </c>
       <c r="B587" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C587" s="4" t="s">
         <v>2</v>
@@ -45034,7 +45034,7 @@
         <v>27</v>
       </c>
       <c r="B588" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C588" s="4" t="s">
         <v>2</v>
@@ -45066,7 +45066,7 @@
         <v>28</v>
       </c>
       <c r="B589" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C589" s="4" t="s">
         <v>2</v>
@@ -45098,7 +45098,7 @@
         <v>29</v>
       </c>
       <c r="B590" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C590" s="4" t="s">
         <v>2</v>
@@ -45130,7 +45130,7 @@
         <v>30</v>
       </c>
       <c r="B591" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C591" s="4" t="s">
         <v>2</v>
@@ -45162,7 +45162,7 @@
         <v>0</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C592" s="2" t="s">
         <v>2</v>
@@ -45194,7 +45194,7 @@
         <v>4</v>
       </c>
       <c r="B593" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C593" s="4" t="s">
         <v>2</v>
@@ -45226,7 +45226,7 @@
         <v>5</v>
       </c>
       <c r="B594" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C594" s="4" t="s">
         <v>2</v>
@@ -45258,7 +45258,7 @@
         <v>6</v>
       </c>
       <c r="B595" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C595" s="4" t="s">
         <v>2</v>
@@ -45290,7 +45290,7 @@
         <v>7</v>
       </c>
       <c r="B596" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C596" s="4" t="s">
         <v>2</v>
@@ -45322,7 +45322,7 @@
         <v>8</v>
       </c>
       <c r="B597" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C597" s="4" t="s">
         <v>2</v>
@@ -45354,7 +45354,7 @@
         <v>9</v>
       </c>
       <c r="B598" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C598" s="4" t="s">
         <v>2</v>
@@ -45386,7 +45386,7 @@
         <v>10</v>
       </c>
       <c r="B599" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C599" s="4" t="s">
         <v>2</v>
@@ -45418,7 +45418,7 @@
         <v>11</v>
       </c>
       <c r="B600" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C600" s="4" t="s">
         <v>2</v>
@@ -45450,7 +45450,7 @@
         <v>12</v>
       </c>
       <c r="B601" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C601" s="4" t="s">
         <v>2</v>
@@ -45482,7 +45482,7 @@
         <v>13</v>
       </c>
       <c r="B602" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C602" s="4" t="s">
         <v>2</v>
@@ -45514,7 +45514,7 @@
         <v>14</v>
       </c>
       <c r="B603" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C603" s="4" t="s">
         <v>2</v>
@@ -45546,7 +45546,7 @@
         <v>15</v>
       </c>
       <c r="B604" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C604" s="4" t="s">
         <v>2</v>
@@ -45578,7 +45578,7 @@
         <v>16</v>
       </c>
       <c r="B605" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C605" s="4" t="s">
         <v>2</v>
@@ -45610,7 +45610,7 @@
         <v>17</v>
       </c>
       <c r="B606" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C606" s="4" t="s">
         <v>2</v>
@@ -45642,7 +45642,7 @@
         <v>18</v>
       </c>
       <c r="B607" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C607" s="4" t="s">
         <v>2</v>
@@ -45674,7 +45674,7 @@
         <v>19</v>
       </c>
       <c r="B608" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C608" s="4" t="s">
         <v>2</v>
@@ -45706,7 +45706,7 @@
         <v>20</v>
       </c>
       <c r="B609" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C609" s="4" t="s">
         <v>2</v>
@@ -45738,7 +45738,7 @@
         <v>21</v>
       </c>
       <c r="B610" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C610" s="4" t="s">
         <v>2</v>
@@ -45770,7 +45770,7 @@
         <v>22</v>
       </c>
       <c r="B611" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C611" s="4" t="s">
         <v>2</v>
@@ -45802,7 +45802,7 @@
         <v>23</v>
       </c>
       <c r="B612" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C612" s="4" t="s">
         <v>2</v>
@@ -45834,7 +45834,7 @@
         <v>24</v>
       </c>
       <c r="B613" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C613" s="4" t="s">
         <v>2</v>
@@ -45866,7 +45866,7 @@
         <v>25</v>
       </c>
       <c r="B614" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C614" s="4" t="s">
         <v>2</v>
@@ -45898,7 +45898,7 @@
         <v>26</v>
       </c>
       <c r="B615" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C615" s="4" t="s">
         <v>2</v>
@@ -45930,7 +45930,7 @@
         <v>27</v>
       </c>
       <c r="B616" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C616" s="4" t="s">
         <v>2</v>
@@ -45962,7 +45962,7 @@
         <v>28</v>
       </c>
       <c r="B617" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C617" s="4" t="s">
         <v>2</v>
@@ -45994,7 +45994,7 @@
         <v>29</v>
       </c>
       <c r="B618" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C618" s="4" t="s">
         <v>2</v>
@@ -46026,7 +46026,7 @@
         <v>30</v>
       </c>
       <c r="B619" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C619" s="4" t="s">
         <v>2</v>
@@ -46058,7 +46058,7 @@
         <v>0</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C620" s="2" t="s">
         <v>2</v>
@@ -46090,7 +46090,7 @@
         <v>4</v>
       </c>
       <c r="B621" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C621" s="4" t="s">
         <v>2</v>
@@ -46122,7 +46122,7 @@
         <v>5</v>
       </c>
       <c r="B622" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C622" s="4" t="s">
         <v>2</v>
@@ -46154,7 +46154,7 @@
         <v>6</v>
       </c>
       <c r="B623" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C623" s="4" t="s">
         <v>2</v>
@@ -46186,7 +46186,7 @@
         <v>7</v>
       </c>
       <c r="B624" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C624" s="4" t="s">
         <v>2</v>
@@ -46218,7 +46218,7 @@
         <v>8</v>
       </c>
       <c r="B625" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C625" s="4" t="s">
         <v>2</v>
@@ -46250,7 +46250,7 @@
         <v>9</v>
       </c>
       <c r="B626" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C626" s="4" t="s">
         <v>2</v>
@@ -46282,7 +46282,7 @@
         <v>10</v>
       </c>
       <c r="B627" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C627" s="4" t="s">
         <v>2</v>
@@ -46314,7 +46314,7 @@
         <v>11</v>
       </c>
       <c r="B628" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C628" s="4" t="s">
         <v>2</v>
@@ -46346,7 +46346,7 @@
         <v>12</v>
       </c>
       <c r="B629" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C629" s="4" t="s">
         <v>2</v>
@@ -46378,7 +46378,7 @@
         <v>13</v>
       </c>
       <c r="B630" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C630" s="4" t="s">
         <v>2</v>
@@ -46410,7 +46410,7 @@
         <v>14</v>
       </c>
       <c r="B631" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C631" s="4" t="s">
         <v>2</v>
@@ -46442,7 +46442,7 @@
         <v>15</v>
       </c>
       <c r="B632" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C632" s="4" t="s">
         <v>2</v>
@@ -46474,7 +46474,7 @@
         <v>16</v>
       </c>
       <c r="B633" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C633" s="4" t="s">
         <v>2</v>
@@ -46506,7 +46506,7 @@
         <v>17</v>
       </c>
       <c r="B634" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C634" s="4" t="s">
         <v>2</v>
@@ -46538,7 +46538,7 @@
         <v>18</v>
       </c>
       <c r="B635" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C635" s="4" t="s">
         <v>2</v>
@@ -46570,7 +46570,7 @@
         <v>19</v>
       </c>
       <c r="B636" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C636" s="4" t="s">
         <v>2</v>
@@ -46602,7 +46602,7 @@
         <v>20</v>
       </c>
       <c r="B637" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C637" s="4" t="s">
         <v>2</v>
@@ -46634,7 +46634,7 @@
         <v>21</v>
       </c>
       <c r="B638" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C638" s="4" t="s">
         <v>2</v>
@@ -46666,7 +46666,7 @@
         <v>22</v>
       </c>
       <c r="B639" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C639" s="4" t="s">
         <v>2</v>
@@ -46698,7 +46698,7 @@
         <v>23</v>
       </c>
       <c r="B640" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C640" s="4" t="s">
         <v>2</v>
@@ -46730,7 +46730,7 @@
         <v>24</v>
       </c>
       <c r="B641" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C641" s="4" t="s">
         <v>2</v>
@@ -46762,7 +46762,7 @@
         <v>25</v>
       </c>
       <c r="B642" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C642" s="4" t="s">
         <v>2</v>
@@ -46794,7 +46794,7 @@
         <v>26</v>
       </c>
       <c r="B643" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C643" s="4" t="s">
         <v>2</v>
@@ -46826,7 +46826,7 @@
         <v>27</v>
       </c>
       <c r="B644" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C644" s="4" t="s">
         <v>2</v>
@@ -46858,7 +46858,7 @@
         <v>28</v>
       </c>
       <c r="B645" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C645" s="4" t="s">
         <v>2</v>
@@ -46890,7 +46890,7 @@
         <v>29</v>
       </c>
       <c r="B646" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C646" s="4" t="s">
         <v>2</v>
@@ -46922,7 +46922,7 @@
         <v>30</v>
       </c>
       <c r="B647" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C647" s="4" t="s">
         <v>2</v>
@@ -46954,7 +46954,7 @@
         <v>0</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C648" s="2" t="s">
         <v>2</v>
@@ -46986,7 +46986,7 @@
         <v>4</v>
       </c>
       <c r="B649" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C649" s="4" t="s">
         <v>2</v>
@@ -47018,7 +47018,7 @@
         <v>5</v>
       </c>
       <c r="B650" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C650" s="4" t="s">
         <v>2</v>
@@ -47050,7 +47050,7 @@
         <v>6</v>
       </c>
       <c r="B651" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C651" s="4" t="s">
         <v>2</v>
@@ -47082,7 +47082,7 @@
         <v>7</v>
       </c>
       <c r="B652" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C652" s="4" t="s">
         <v>2</v>
@@ -47114,7 +47114,7 @@
         <v>8</v>
       </c>
       <c r="B653" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C653" s="4" t="s">
         <v>2</v>
@@ -47146,7 +47146,7 @@
         <v>9</v>
       </c>
       <c r="B654" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C654" s="4" t="s">
         <v>2</v>
@@ -47178,7 +47178,7 @@
         <v>10</v>
       </c>
       <c r="B655" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C655" s="4" t="s">
         <v>2</v>
@@ -47210,7 +47210,7 @@
         <v>11</v>
       </c>
       <c r="B656" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C656" s="4" t="s">
         <v>2</v>
@@ -47242,7 +47242,7 @@
         <v>12</v>
       </c>
       <c r="B657" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C657" s="4" t="s">
         <v>2</v>
@@ -47274,7 +47274,7 @@
         <v>13</v>
       </c>
       <c r="B658" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C658" s="4" t="s">
         <v>2</v>
@@ -47306,7 +47306,7 @@
         <v>14</v>
       </c>
       <c r="B659" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C659" s="4" t="s">
         <v>2</v>
@@ -47338,7 +47338,7 @@
         <v>15</v>
       </c>
       <c r="B660" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C660" s="4" t="s">
         <v>2</v>
@@ -47370,7 +47370,7 @@
         <v>16</v>
       </c>
       <c r="B661" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C661" s="4" t="s">
         <v>2</v>
@@ -47402,7 +47402,7 @@
         <v>17</v>
       </c>
       <c r="B662" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C662" s="4" t="s">
         <v>2</v>
@@ -47434,7 +47434,7 @@
         <v>18</v>
       </c>
       <c r="B663" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C663" s="4" t="s">
         <v>2</v>
@@ -47466,7 +47466,7 @@
         <v>19</v>
       </c>
       <c r="B664" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C664" s="4" t="s">
         <v>2</v>
@@ -47498,7 +47498,7 @@
         <v>20</v>
       </c>
       <c r="B665" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C665" s="4" t="s">
         <v>2</v>
@@ -47530,7 +47530,7 @@
         <v>21</v>
       </c>
       <c r="B666" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C666" s="4" t="s">
         <v>2</v>
@@ -47562,7 +47562,7 @@
         <v>22</v>
       </c>
       <c r="B667" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C667" s="4" t="s">
         <v>2</v>
@@ -47594,7 +47594,7 @@
         <v>23</v>
       </c>
       <c r="B668" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C668" s="4" t="s">
         <v>2</v>
@@ -47626,7 +47626,7 @@
         <v>24</v>
       </c>
       <c r="B669" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C669" s="4" t="s">
         <v>2</v>
@@ -47658,7 +47658,7 @@
         <v>25</v>
       </c>
       <c r="B670" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C670" s="4" t="s">
         <v>2</v>
@@ -47690,7 +47690,7 @@
         <v>26</v>
       </c>
       <c r="B671" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C671" s="4" t="s">
         <v>2</v>
@@ -47722,7 +47722,7 @@
         <v>27</v>
       </c>
       <c r="B672" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C672" s="4" t="s">
         <v>2</v>
@@ -47754,7 +47754,7 @@
         <v>28</v>
       </c>
       <c r="B673" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C673" s="4" t="s">
         <v>2</v>
@@ -47786,7 +47786,7 @@
         <v>29</v>
       </c>
       <c r="B674" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C674" s="4" t="s">
         <v>2</v>
@@ -47818,7 +47818,7 @@
         <v>30</v>
       </c>
       <c r="B675" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C675" s="4" t="s">
         <v>2</v>
@@ -47867,7 +47867,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -47915,10 +47915,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -47944,10 +47944,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -47973,12 +47973,12 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -47996,18 +47996,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>